<commit_message>
right back at you wargen
</commit_message>
<xml_diff>
--- a/F20/STAT411/STATS4.xlsx
+++ b/F20/STAT411/STATS4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\SchoolProjects\F20\STAT411\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/warg/Desktop/github/schoolProjects/F20/STAT411/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F2C016-E6D7-4FDF-889F-2261C406C95F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E53552F-3FE6-1241-BA2D-77DE52326153}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{83F9DAE8-36B0-4308-9B2D-424F7D0F621D}"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="28800" windowHeight="16440" activeTab="1" xr2:uid="{83F9DAE8-36B0-4308-9B2D-424F7D0F621D}"/>
   </bookViews>
   <sheets>
     <sheet name="Chapter 11" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="60">
   <si>
     <t>a = 1 - c</t>
   </si>
@@ -210,6 +210,12 @@
   </si>
   <si>
     <t>mj</t>
+  </si>
+  <si>
+    <t>take smaller of the two for crit</t>
+  </si>
+  <si>
+    <t>decimal is a and percent is a/2</t>
   </si>
 </sst>
 </file>
@@ -218,9 +224,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,6 +246,18 @@
       <color rgb="FF45494D"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="17"/>
+      <color rgb="FF4D4D4D"/>
+      <name val="STIXGeneral-Regular"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -268,7 +286,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -279,9 +297,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -297,6 +321,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>272724</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{318F5336-A810-984B-9604-1CC5A4A900D1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7835900" y="3822700"/>
+          <a:ext cx="7772400" cy="1326824"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -598,18 +671,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C8478AB-05BE-4582-B00F-80C549F49589}">
   <dimension ref="A1:AF57"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:R57"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="U21" sqref="U21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="10" max="10" width="10.5703125" customWidth="1"/>
-    <col min="20" max="20" width="10.85546875" customWidth="1"/>
-    <col min="21" max="21" width="50.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10.5" customWidth="1"/>
+    <col min="20" max="20" width="10.83203125" customWidth="1"/>
+    <col min="21" max="21" width="50.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" ht="80">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
@@ -637,7 +710,7 @@
       <c r="R1">
         <v>99</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="9" t="s">
         <v>28</v>
       </c>
       <c r="W1">
@@ -671,7 +744,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -742,9 +815,9 @@
         <v>7.8789999999999996</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>7.1</v>
+    <row r="3" spans="1:32" ht="28">
+      <c r="A3" s="10">
+        <v>104</v>
       </c>
       <c r="D3">
         <v>0.8</v>
@@ -781,7 +854,7 @@
         <v>63.656999999999996</v>
       </c>
       <c r="T3">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="V3">
         <v>2</v>
@@ -817,7 +890,7 @@
         <v>10.597</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32">
       <c r="D4">
         <v>0.85</v>
       </c>
@@ -882,7 +955,7 @@
         <v>12.837999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -956,9 +1029,9 @@
         <v>14.86</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>27</v>
+    <row r="6" spans="1:32" ht="28">
+      <c r="A6" s="10">
+        <v>60</v>
       </c>
       <c r="D6">
         <v>0.95</v>
@@ -991,12 +1064,12 @@
         <v>4.6040000000000001</v>
       </c>
       <c r="T6">
-        <f>0.22*0.22</f>
-        <v>4.8399999999999999E-2</v>
+        <f>16.6158*16.6158</f>
+        <v>276.08480964</v>
       </c>
       <c r="U6" s="1">
         <f>(T3-1)*T6/T9</f>
-        <v>27.103999999999999</v>
+        <v>60.738658120800004</v>
       </c>
       <c r="V6">
         <v>5</v>
@@ -1032,7 +1105,7 @@
         <v>16.75</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32">
       <c r="D7">
         <v>0.96</v>
       </c>
@@ -1097,7 +1170,7 @@
         <v>18.547999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1168,9 +1241,9 @@
         <v>20.277999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>7</v>
+    <row r="9" spans="1:32" ht="28">
+      <c r="A9" s="10">
+        <v>102</v>
       </c>
       <c r="D9">
         <v>0.99</v>
@@ -1203,7 +1276,7 @@
         <v>3.4990000000000001</v>
       </c>
       <c r="T9">
-        <v>2.5000000000000001E-2</v>
+        <v>100</v>
       </c>
       <c r="V9">
         <v>8</v>
@@ -1239,7 +1312,7 @@
         <v>21.954999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32">
       <c r="M10">
         <v>8</v>
       </c>
@@ -1292,7 +1365,7 @@
         <v>23.588999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1354,15 +1427,15 @@
         <v>25.187999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32">
       <c r="A12">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C12" s="1">
         <f>(A9-A3)/(A12/SQRT(A6))</f>
-        <v>-0.51961524227066136</v>
-      </c>
-      <c r="G12">
+        <v>-1.9364916731037087</v>
+      </c>
+      <c r="G12" s="4">
         <v>11.4</v>
       </c>
       <c r="H12" t="s">
@@ -1420,7 +1493,7 @@
         <v>26.757000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32">
       <c r="G13" t="s">
         <v>23</v>
       </c>
@@ -1442,7 +1515,7 @@
       <c r="R13">
         <v>3.1059999999999999</v>
       </c>
-      <c r="U13" t="s">
+      <c r="U13" s="4" t="s">
         <v>34</v>
       </c>
       <c r="V13">
@@ -1479,12 +1552,12 @@
         <v>28.3</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32">
       <c r="A14" t="s">
         <v>7</v>
       </c>
       <c r="G14">
-        <v>0.7</v>
+        <v>0.64</v>
       </c>
       <c r="M14">
         <v>12</v>
@@ -1544,7 +1617,7 @@
         <v>29.818999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32">
       <c r="A15">
         <v>2.0499999999999998</v>
       </c>
@@ -1607,7 +1680,7 @@
         <v>31.318999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32">
       <c r="G16" t="s">
         <v>24</v>
       </c>
@@ -1663,12 +1736,12 @@
         <v>32.801000000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:32">
       <c r="A17" t="s">
         <v>9</v>
       </c>
       <c r="G17">
-        <v>0.75</v>
+        <v>0.61</v>
       </c>
       <c r="M17">
         <v>15</v>
@@ -1728,7 +1801,7 @@
         <v>34.267000000000003</v>
       </c>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:32">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -1790,7 +1863,7 @@
         <v>35.718000000000004</v>
       </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:32">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -1849,9 +1922,9 @@
         <v>37.155999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:32">
       <c r="G20">
-        <v>180</v>
+        <v>1100</v>
       </c>
       <c r="M20">
         <v>18</v>
@@ -1908,7 +1981,7 @@
         <v>38.582000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:32">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -1967,7 +2040,7 @@
         <v>39.997</v>
       </c>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:32">
       <c r="G22" t="s">
         <v>8</v>
       </c>
@@ -2023,7 +2096,7 @@
         <v>41.401000000000003</v>
       </c>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:32">
       <c r="A23" s="4">
         <v>11.3</v>
       </c>
@@ -2032,7 +2105,7 @@
       </c>
       <c r="G23" s="5">
         <f>(G14-G17)/SQRT((G17*(1-G17))/G20)</f>
-        <v>-1.5491933384829684</v>
+        <v>2.0399540088280612</v>
       </c>
       <c r="M23">
         <v>21</v>
@@ -2089,7 +2162,7 @@
         <v>42.795999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:32">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -2151,13 +2224,13 @@
         <v>44.180999999999997</v>
       </c>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:32">
       <c r="A25">
-        <v>820</v>
+        <v>530</v>
       </c>
       <c r="C25">
         <f>A25-(A28*(A31/SQRT(A34)))</f>
-        <v>798.91200000000003</v>
+        <v>508.08749999999998</v>
       </c>
       <c r="G25" t="s">
         <v>26</v>
@@ -2214,10 +2287,10 @@
         <v>45.558999999999997</v>
       </c>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:32">
       <c r="C26">
         <f>A25+(A28*(A31/SQRT(A34)))</f>
-        <v>841.08799999999997</v>
+        <v>551.91250000000002</v>
       </c>
       <c r="G26" t="s">
         <v>27</v>
@@ -2274,7 +2347,7 @@
         <v>46.927999999999997</v>
       </c>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:32">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -2330,9 +2403,9 @@
         <v>48.29</v>
       </c>
     </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:32">
       <c r="A28">
-        <v>1.3180000000000001</v>
+        <v>1.7529999999999999</v>
       </c>
       <c r="M28">
         <v>26</v>
@@ -2386,7 +2459,7 @@
         <v>49.645000000000003</v>
       </c>
     </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:32">
       <c r="M29">
         <v>27</v>
       </c>
@@ -2440,7 +2513,7 @@
         <v>50.993000000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:32">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -2496,9 +2569,9 @@
         <v>52.335999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:32">
       <c r="A31">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="M31">
         <v>29</v>
@@ -2552,7 +2625,7 @@
         <v>53.671999999999997</v>
       </c>
     </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:32">
       <c r="M32">
         <v>30</v>
       </c>
@@ -2605,7 +2678,7 @@
         <v>66.766000000000005</v>
       </c>
     </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:32">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -2661,9 +2734,9 @@
         <v>79.489999999999995</v>
       </c>
     </row>
-    <row r="34" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:32">
       <c r="A34">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="M34">
         <v>32</v>
@@ -2717,7 +2790,7 @@
         <v>91.951999999999998</v>
       </c>
     </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:32">
       <c r="M35">
         <v>34</v>
       </c>
@@ -2770,7 +2843,7 @@
         <v>104.215</v>
       </c>
     </row>
-    <row r="36" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:32">
       <c r="M36">
         <v>36</v>
       </c>
@@ -2823,7 +2896,7 @@
         <v>116.321</v>
       </c>
     </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:32">
       <c r="M37">
         <v>38</v>
       </c>
@@ -2876,7 +2949,7 @@
         <v>128.29900000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:32">
       <c r="M38">
         <v>40</v>
       </c>
@@ -2929,7 +3002,7 @@
         <v>140.16900000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:32">
       <c r="M39">
         <v>45</v>
       </c>
@@ -2949,7 +3022,7 @@
         <v>2.69</v>
       </c>
     </row>
-    <row r="40" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:32">
       <c r="M40">
         <v>50</v>
       </c>
@@ -2969,7 +3042,7 @@
         <v>2.6779999999999999</v>
       </c>
     </row>
-    <row r="41" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:32">
       <c r="M41">
         <v>55</v>
       </c>
@@ -2989,7 +3062,7 @@
         <v>2.6680000000000001</v>
       </c>
     </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:32">
       <c r="M42">
         <v>60</v>
       </c>
@@ -3009,7 +3082,7 @@
         <v>2.66</v>
       </c>
     </row>
-    <row r="43" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:32">
       <c r="M43">
         <v>65</v>
       </c>
@@ -3029,7 +3102,7 @@
         <v>2.6539999999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:32">
       <c r="M44">
         <v>70</v>
       </c>
@@ -3049,7 +3122,7 @@
         <v>2.6480000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:32">
       <c r="M45">
         <v>75</v>
       </c>
@@ -3069,7 +3142,7 @@
         <v>2.6429999999999998</v>
       </c>
     </row>
-    <row r="46" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:32">
       <c r="M46">
         <v>80</v>
       </c>
@@ -3089,7 +3162,7 @@
         <v>2.6389999999999998</v>
       </c>
     </row>
-    <row r="47" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:32">
       <c r="M47">
         <v>90</v>
       </c>
@@ -3109,7 +3182,7 @@
         <v>2.6320000000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:32">
       <c r="M48">
         <v>100</v>
       </c>
@@ -3129,7 +3202,7 @@
         <v>2.6259999999999999</v>
       </c>
     </row>
-    <row r="49" spans="13:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="13:18">
       <c r="M49">
         <v>120</v>
       </c>
@@ -3149,7 +3222,7 @@
         <v>2.617</v>
       </c>
     </row>
-    <row r="50" spans="13:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="13:18">
       <c r="M50">
         <v>200</v>
       </c>
@@ -3169,7 +3242,7 @@
         <v>2.601</v>
       </c>
     </row>
-    <row r="51" spans="13:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="13:18">
       <c r="M51">
         <v>300</v>
       </c>
@@ -3189,7 +3262,7 @@
         <v>2.5920000000000001</v>
       </c>
     </row>
-    <row r="52" spans="13:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="13:18">
       <c r="M52">
         <v>400</v>
       </c>
@@ -3209,7 +3282,7 @@
         <v>2.5880000000000001</v>
       </c>
     </row>
-    <row r="53" spans="13:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="13:18">
       <c r="M53">
         <v>500</v>
       </c>
@@ -3229,7 +3302,7 @@
         <v>2.5859999999999999</v>
       </c>
     </row>
-    <row r="54" spans="13:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="13:18">
       <c r="M54">
         <v>750</v>
       </c>
@@ -3249,7 +3322,7 @@
         <v>2.5819999999999999</v>
       </c>
     </row>
-    <row r="55" spans="13:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="13:18">
       <c r="M55">
         <v>1000</v>
       </c>
@@ -3269,7 +3342,7 @@
         <v>2.581</v>
       </c>
     </row>
-    <row r="56" spans="13:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="13:18">
       <c r="M56">
         <v>2000</v>
       </c>
@@ -3289,7 +3362,7 @@
         <v>2.5779999999999998</v>
       </c>
     </row>
-    <row r="57" spans="13:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="13:18">
       <c r="M57" t="s">
         <v>16</v>
       </c>
@@ -3319,18 +3392,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6D6EBE5-4431-4874-A2E4-BBFED1A3301F}">
   <dimension ref="A1:P76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16">
       <c r="A1" s="7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -3344,7 +3420,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -3370,16 +3446,16 @@
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>79</v>
-      </c>
-      <c r="B4">
-        <v>75</v>
+    <row r="4" spans="1:16" ht="28">
+      <c r="A4" s="10">
+        <v>68</v>
+      </c>
+      <c r="B4" s="10">
+        <v>31</v>
       </c>
       <c r="D4" s="5">
         <f>((A7-B7)-(A10-B10))/SQRT((A13*A13/A4)+(B13*B13/B4))</f>
-        <v>4.1351622821319962</v>
+        <v>-1.2200279593608314</v>
       </c>
       <c r="F4">
         <v>0.8</v>
@@ -3400,7 +3476,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16">
       <c r="F5">
         <v>0.85</v>
       </c>
@@ -3420,7 +3496,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -3449,16 +3525,16 @@
         <v>129</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>87</v>
-      </c>
-      <c r="B7">
-        <v>83</v>
+    <row r="7" spans="1:16" ht="28">
+      <c r="A7" s="11">
+        <v>40046</v>
+      </c>
+      <c r="B7" s="11">
+        <v>41126</v>
       </c>
       <c r="D7">
         <f>SQRT((A13*A13/A4)+(B13*B13/B4))</f>
-        <v>0.96731391106075049</v>
+        <v>885.22561447346527</v>
       </c>
       <c r="F7">
         <v>0.95</v>
@@ -3479,7 +3555,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16">
       <c r="F8">
         <v>0.96</v>
       </c>
@@ -3502,7 +3578,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -3531,7 +3607,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16">
       <c r="A10">
         <v>0</v>
       </c>
@@ -3540,7 +3616,7 @@
       </c>
       <c r="D10" s="6">
         <f>A7-B7-A16*SQRT((A13*A13/A4)+(B13*B13/B4))</f>
-        <v>2.7618381938422392</v>
+        <v>-2536.1961358088502</v>
       </c>
       <c r="F10">
         <v>0.99</v>
@@ -3561,7 +3637,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16">
       <c r="L11">
         <v>128</v>
       </c>
@@ -3569,7 +3645,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -3586,17 +3662,22 @@
         <v>129</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>6</v>
-      </c>
-      <c r="B13">
-        <v>6</v>
+    <row r="13" spans="1:16" ht="28">
+      <c r="A13" s="10">
+        <v>2087</v>
+      </c>
+      <c r="B13" s="10">
+        <v>4723</v>
       </c>
       <c r="D13" s="6">
         <f>A7-B7+A16*SQRT((A13*A13/A4)+(B13*B13/B4))</f>
-        <v>5.2381618061577608</v>
-      </c>
+        <v>376.19613580885039</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
       <c r="L13">
         <v>127</v>
       </c>
@@ -3604,12 +3685,12 @@
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16">
       <c r="M14">
         <v>132</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -3617,9 +3698,9 @@
         <v>131</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>1.28</v>
+    <row r="16" spans="1:16">
+      <c r="A16" s="12">
+        <v>1.645</v>
       </c>
       <c r="L16">
         <f>AVERAGE(L3:L13)</f>
@@ -3630,18 +3711,18 @@
         <v>129.53846153846155</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12">
       <c r="L17">
         <f>M16-L16</f>
         <v>0.99300699300701467</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12">
       <c r="A18" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12">
       <c r="A19" t="s">
         <v>40</v>
       </c>
@@ -3649,7 +3730,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -3675,16 +3756,16 @@
         <v>99</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>53</v>
-      </c>
-      <c r="B21">
-        <v>57</v>
+    <row r="21" spans="1:12" ht="28">
+      <c r="A21" s="10">
+        <v>7</v>
+      </c>
+      <c r="B21" s="10">
+        <v>7</v>
       </c>
       <c r="D21" s="8">
         <f>SQRT(((A21-1)*A30*A30+(B21-1)*B30*B30)/(A21+B21-2))</f>
-        <v>36.286376384410602</v>
+        <v>23.717082451262844</v>
       </c>
       <c r="G21">
         <v>0.1</v>
@@ -3702,7 +3783,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12">
       <c r="F22">
         <v>1</v>
       </c>
@@ -3722,7 +3803,7 @@
         <v>63.656999999999996</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12">
       <c r="A23" t="s">
         <v>45</v>
       </c>
@@ -3751,16 +3832,16 @@
         <v>9.9250000000000007</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>505</v>
-      </c>
-      <c r="B24">
-        <v>499</v>
+    <row r="24" spans="1:12" ht="28">
+      <c r="A24" s="10">
+        <v>197</v>
+      </c>
+      <c r="B24" s="10">
+        <v>181</v>
       </c>
       <c r="D24" s="1">
         <f>(A24-B24-A27-B27)/(D21*SQRT(1/A21+1/B21))</f>
-        <v>0.86653611841408573</v>
+        <v>1.2620970203945847</v>
       </c>
       <c r="F24">
         <v>3</v>
@@ -3781,7 +3862,7 @@
         <v>5.8410000000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12">
       <c r="F25">
         <v>4</v>
       </c>
@@ -3801,7 +3882,7 @@
         <v>4.6040000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12">
       <c r="A26" t="s">
         <v>46</v>
       </c>
@@ -3830,7 +3911,7 @@
         <v>4.032</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12">
       <c r="A27">
         <v>0</v>
       </c>
@@ -3839,7 +3920,7 @@
       </c>
       <c r="D27" s="5">
         <f>SQRT((A30*A30/A21)+(B30*B30/B21))</f>
-        <v>6.9722258379031015</v>
+        <v>12.677313820927749</v>
       </c>
       <c r="F27">
         <v>6</v>
@@ -3860,7 +3941,7 @@
         <v>3.7069999999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12">
       <c r="F28">
         <v>7</v>
       </c>
@@ -3880,7 +3961,7 @@
         <v>3.4990000000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -3909,16 +3990,16 @@
         <v>3.355</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>39.700000000000003</v>
-      </c>
-      <c r="B30">
-        <v>32.799999999999997</v>
-      </c>
-      <c r="D30" s="8">
+    <row r="30" spans="1:12" ht="28">
+      <c r="A30" s="10">
+        <v>30</v>
+      </c>
+      <c r="B30" s="10">
+        <v>15</v>
+      </c>
+      <c r="D30" s="5">
         <f>A24-B24-A33*D27</f>
-        <v>-5.9294784086522068</v>
+        <v>-15.021386919810201</v>
       </c>
       <c r="F30">
         <v>9</v>
@@ -3939,7 +4020,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12">
       <c r="F31">
         <v>10</v>
       </c>
@@ -3959,7 +4040,7 @@
         <v>3.169</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12">
       <c r="A32" t="s">
         <v>48</v>
       </c>
@@ -3985,13 +4066,13 @@
         <v>3.1059999999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11">
       <c r="A33">
-        <v>1.7110000000000001</v>
-      </c>
-      <c r="D33" s="8">
+        <v>2.4470000000000001</v>
+      </c>
+      <c r="D33" s="5">
         <f>A24-B24+A33*D27</f>
-        <v>17.929478408652209</v>
+        <v>47.021386919810197</v>
       </c>
       <c r="F33">
         <v>12</v>
@@ -4012,7 +4093,7 @@
         <v>3.0550000000000002</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11">
       <c r="F34">
         <v>13</v>
       </c>
@@ -4032,7 +4113,10 @@
         <v>3.012</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11">
+      <c r="A35" t="s">
+        <v>58</v>
+      </c>
       <c r="D35" t="s">
         <v>54</v>
       </c>
@@ -4055,10 +4139,10 @@
         <v>2.9769999999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11">
       <c r="D36" s="8">
         <f>D21*SQRT(1/A21+1/B21)</f>
-        <v>6.924119921257363</v>
+        <v>12.677313820927749</v>
       </c>
       <c r="F36">
         <v>15</v>
@@ -4079,7 +4163,7 @@
         <v>2.9470000000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11">
       <c r="F37">
         <v>16</v>
       </c>
@@ -4099,7 +4183,7 @@
         <v>2.9209999999999998</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11">
       <c r="D38" t="s">
         <v>55</v>
       </c>
@@ -4122,10 +4206,10 @@
         <v>2.8980000000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11">
       <c r="D39" s="8">
         <f>A24-B24-A33*D36</f>
-        <v>-5.8471691852713494</v>
+        <v>-15.021386919810201</v>
       </c>
       <c r="F39">
         <v>18</v>
@@ -4146,7 +4230,7 @@
         <v>2.8780000000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11">
       <c r="F40">
         <v>19</v>
       </c>
@@ -4166,7 +4250,7 @@
         <v>2.8610000000000002</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11">
       <c r="D41" t="s">
         <v>56</v>
       </c>
@@ -4189,10 +4273,10 @@
         <v>2.8450000000000002</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11">
       <c r="D42" s="8">
         <f>A24-B24+A33*D36</f>
-        <v>17.847169185271348</v>
+        <v>47.021386919810197</v>
       </c>
       <c r="F42">
         <v>21</v>
@@ -4213,7 +4297,7 @@
         <v>2.831</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11">
       <c r="F43">
         <v>22</v>
       </c>
@@ -4233,7 +4317,7 @@
         <v>2.819</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11">
       <c r="F44">
         <v>23</v>
       </c>
@@ -4253,7 +4337,7 @@
         <v>2.8069999999999999</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11">
       <c r="F45">
         <v>24</v>
       </c>
@@ -4273,7 +4357,7 @@
         <v>2.7970000000000002</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11">
       <c r="F46">
         <v>25</v>
       </c>
@@ -4293,7 +4377,7 @@
         <v>2.7869999999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11">
       <c r="F47">
         <v>26</v>
       </c>
@@ -4313,7 +4397,7 @@
         <v>2.7789999999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11">
       <c r="F48">
         <v>27</v>
       </c>
@@ -4333,7 +4417,7 @@
         <v>2.7709999999999999</v>
       </c>
     </row>
-    <row r="49" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="6:11">
       <c r="F49">
         <v>28</v>
       </c>
@@ -4353,7 +4437,7 @@
         <v>2.7629999999999999</v>
       </c>
     </row>
-    <row r="50" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="6:11">
       <c r="F50">
         <v>29</v>
       </c>
@@ -4373,7 +4457,7 @@
         <v>2.7559999999999998</v>
       </c>
     </row>
-    <row r="51" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="6:11">
       <c r="F51">
         <v>30</v>
       </c>
@@ -4393,7 +4477,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="52" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="6:11">
       <c r="F52">
         <v>31</v>
       </c>
@@ -4413,7 +4497,7 @@
         <v>2.7440000000000002</v>
       </c>
     </row>
-    <row r="53" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="6:11">
       <c r="F53">
         <v>32</v>
       </c>
@@ -4433,7 +4517,7 @@
         <v>2.738</v>
       </c>
     </row>
-    <row r="54" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="6:11">
       <c r="F54">
         <v>34</v>
       </c>
@@ -4453,7 +4537,7 @@
         <v>2.7280000000000002</v>
       </c>
     </row>
-    <row r="55" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="6:11">
       <c r="F55">
         <v>36</v>
       </c>
@@ -4473,7 +4557,7 @@
         <v>2.7189999999999999</v>
       </c>
     </row>
-    <row r="56" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="6:11">
       <c r="F56">
         <v>38</v>
       </c>
@@ -4493,7 +4577,7 @@
         <v>2.7120000000000002</v>
       </c>
     </row>
-    <row r="57" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="6:11">
       <c r="F57">
         <v>40</v>
       </c>
@@ -4513,7 +4597,7 @@
         <v>2.7040000000000002</v>
       </c>
     </row>
-    <row r="58" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="6:11">
       <c r="F58">
         <v>45</v>
       </c>
@@ -4533,7 +4617,7 @@
         <v>2.69</v>
       </c>
     </row>
-    <row r="59" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="6:11">
       <c r="F59">
         <v>50</v>
       </c>
@@ -4553,7 +4637,7 @@
         <v>2.6779999999999999</v>
       </c>
     </row>
-    <row r="60" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="6:11">
       <c r="F60">
         <v>55</v>
       </c>
@@ -4573,7 +4657,7 @@
         <v>2.6680000000000001</v>
       </c>
     </row>
-    <row r="61" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="6:11">
       <c r="F61">
         <v>60</v>
       </c>
@@ -4593,7 +4677,7 @@
         <v>2.66</v>
       </c>
     </row>
-    <row r="62" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="6:11">
       <c r="F62">
         <v>65</v>
       </c>
@@ -4613,7 +4697,7 @@
         <v>2.6539999999999999</v>
       </c>
     </row>
-    <row r="63" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="6:11">
       <c r="F63">
         <v>70</v>
       </c>
@@ -4633,7 +4717,7 @@
         <v>2.6480000000000001</v>
       </c>
     </row>
-    <row r="64" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="6:11">
       <c r="F64">
         <v>75</v>
       </c>
@@ -4653,7 +4737,7 @@
         <v>2.6429999999999998</v>
       </c>
     </row>
-    <row r="65" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="6:11">
       <c r="F65">
         <v>80</v>
       </c>
@@ -4673,7 +4757,7 @@
         <v>2.6389999999999998</v>
       </c>
     </row>
-    <row r="66" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="6:11">
       <c r="F66">
         <v>90</v>
       </c>
@@ -4693,7 +4777,7 @@
         <v>2.6320000000000001</v>
       </c>
     </row>
-    <row r="67" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="6:11">
       <c r="F67">
         <v>100</v>
       </c>
@@ -4713,7 +4797,7 @@
         <v>2.6259999999999999</v>
       </c>
     </row>
-    <row r="68" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="6:11">
       <c r="F68">
         <v>120</v>
       </c>
@@ -4733,7 +4817,7 @@
         <v>2.617</v>
       </c>
     </row>
-    <row r="69" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="6:11">
       <c r="F69">
         <v>200</v>
       </c>
@@ -4753,7 +4837,7 @@
         <v>2.601</v>
       </c>
     </row>
-    <row r="70" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="6:11">
       <c r="F70">
         <v>300</v>
       </c>
@@ -4773,7 +4857,7 @@
         <v>2.5920000000000001</v>
       </c>
     </row>
-    <row r="71" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="6:11">
       <c r="F71">
         <v>400</v>
       </c>
@@ -4793,7 +4877,7 @@
         <v>2.5880000000000001</v>
       </c>
     </row>
-    <row r="72" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="6:11">
       <c r="F72">
         <v>500</v>
       </c>
@@ -4813,7 +4897,7 @@
         <v>2.5859999999999999</v>
       </c>
     </row>
-    <row r="73" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="6:11">
       <c r="F73">
         <v>750</v>
       </c>
@@ -4833,7 +4917,7 @@
         <v>2.5819999999999999</v>
       </c>
     </row>
-    <row r="74" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="6:11">
       <c r="F74">
         <v>1000</v>
       </c>
@@ -4853,7 +4937,7 @@
         <v>2.581</v>
       </c>
     </row>
-    <row r="75" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="6:11">
       <c r="F75">
         <v>2000</v>
       </c>
@@ -4873,7 +4957,7 @@
         <v>2.5779999999999998</v>
       </c>
     </row>
-    <row r="76" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="6:11">
       <c r="F76" t="s">
         <v>16</v>
       </c>
@@ -4896,5 +4980,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>